<commit_message>
fix: Spring reaction. add: Function is_number
</commit_message>
<xml_diff>
--- a/src/examples/excel/matheus_romero.xlsx
+++ b/src/examples/excel/matheus_romero.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developer\PyEngineer\src\examples\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B957F64-6BD7-4764-B246-286ABB6B7C5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B8E686-8261-481D-BDDE-4525BBEE9E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="4" xr2:uid="{17B9D78E-9B11-469E-9BF6-00D2F9C8B7DE}"/>
   </bookViews>
@@ -1388,7 +1388,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1480,11 +1480,11 @@
       <c r="D4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="1">
-        <v>10</v>
-      </c>
-      <c r="F4" s="1">
-        <v>10</v>
+      <c r="E4" s="3">
+        <v>30000000</v>
+      </c>
+      <c r="F4" s="3">
+        <v>30000000</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
fix: Add zero in supports with not fixed.
</commit_message>
<xml_diff>
--- a/src/examples/excel/matheus_romero.xlsx
+++ b/src/examples/excel/matheus_romero.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developer\PyEngineer\src\examples\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B8E686-8261-481D-BDDE-4525BBEE9E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7620AFF-5C5D-4341-8ED2-FC401C11B138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="4" xr2:uid="{17B9D78E-9B11-469E-9BF6-00D2F9C8B7DE}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="81">
   <si>
     <t>E</t>
   </si>
@@ -1388,7 +1388,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1429,13 +1429,13 @@
         <v>33</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>79</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>33</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>33</v>
+        <v>79</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>33</v>
@@ -1471,8 +1471,8 @@
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>33</v>
+      <c r="B4" s="3">
+        <v>30000000</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
ref: Remove old typing
</commit_message>
<xml_diff>
--- a/src/examples/excel/matheus_romero.xlsx
+++ b/src/examples/excel/matheus_romero.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developer\PyEngineer\src\examples\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7620AFF-5C5D-4341-8ED2-FC401C11B138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93490437-64A9-4537-852F-4CF412EC8EC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="4" xr2:uid="{17B9D78E-9B11-469E-9BF6-00D2F9C8B7DE}"/>
   </bookViews>
@@ -1388,7 +1388,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>